<commit_message>
some new ideas in the general higher level card document
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_higher-level_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_higher-level_CC.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47F98BF4-3CA0-4D27-B70C-D11957D665C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD042F06-4391-4F24-8417-4ADCEC662814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="26370" windowHeight="15690"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tactile Tabletop Data - Higher " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="125">
   <si>
     <t>Top Ability Name</t>
   </si>
@@ -368,12 +368,51 @@
   </si>
   <si>
     <t>hand</t>
+  </si>
+  <si>
+    <t>Dempsey Roll</t>
+  </si>
+  <si>
+    <t>something that probably lowers defense more and more each round, but leads to higher damage with each round? And allows for an attack each round? Risk reward thing</t>
+  </si>
+  <si>
+    <t>The Final Nail</t>
+  </si>
+  <si>
+    <t>use a mark to do something cool</t>
+  </si>
+  <si>
+    <t>And the hammer that drove it</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>something also with marks?</t>
+  </si>
+  <si>
+    <t>Tight 5</t>
+  </si>
+  <si>
+    <t>Something using charisma</t>
+  </si>
+  <si>
+    <t>And the winner is…</t>
+  </si>
+  <si>
+    <t>enchant a small container of liquid. When broken over a weapon, the next attack made with that weapon does an additional 1d8 fire damage</t>
+  </si>
+  <si>
+    <t>exhaust</t>
+  </si>
+  <si>
+    <t>Flame Oil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1210,10 +1249,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1840,7 +1881,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -1848,7 +1889,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -1857,6 +1898,73 @@
       </c>
       <c r="F18" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" t="s">
+        <v>117</v>
+      </c>
+      <c r="K20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>